<commit_message>
fix: update reward system
</commit_message>
<xml_diff>
--- a/Kniffel.xlsx
+++ b/Kniffel.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2d5b8c672a84e6c/Dokumente/Git/Kniffel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B05D1B8-8BF1-4EF5-93BA-D5FE73E20C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{1B05D1B8-8BF1-4EF5-93BA-D5FE73E20C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F67741E-5535-4EBE-A76E-2ACA8BB9E338}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="4290" windowWidth="29955" windowHeight="15525" xr2:uid="{AE988D40-45C8-4635-93D3-6D8C6975B537}"/>
+    <workbookView xWindow="6615" yWindow="-45" windowWidth="29955" windowHeight="15525" activeTab="2" xr2:uid="{AE988D40-45C8-4635-93D3-6D8C6975B537}"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Kategorie</t>
   </si>
@@ -119,16 +121,91 @@
   </si>
   <si>
     <t>375</t>
+  </si>
+  <si>
+    <t>ONES</t>
+  </si>
+  <si>
+    <t>TWOS</t>
+  </si>
+  <si>
+    <t>THREES</t>
+  </si>
+  <si>
+    <t>FOURS</t>
+  </si>
+  <si>
+    <t>FIVES</t>
+  </si>
+  <si>
+    <t>SIXES</t>
+  </si>
+  <si>
+    <t>THREE_TIMES</t>
+  </si>
+  <si>
+    <t>FOUR_TIMES</t>
+  </si>
+  <si>
+    <t>FULL_HOUSE</t>
+  </si>
+  <si>
+    <t>SMALL_STREET</t>
+  </si>
+  <si>
+    <t>LARGE_STREET</t>
+  </si>
+  <si>
+    <t>KNIFFEL</t>
+  </si>
+  <si>
+    <t>CHANCE</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Slash</t>
+  </si>
+  <si>
+    <t>Prop5Dice</t>
+  </si>
+  <si>
+    <t>Prop4Dice</t>
+  </si>
+  <si>
+    <t>Prop3Dice</t>
+  </si>
+  <si>
+    <t>Prop2Dice</t>
+  </si>
+  <si>
+    <t>Prop1Dice</t>
+  </si>
+  <si>
+    <t>Example5Dice</t>
+  </si>
+  <si>
+    <t>Example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,13 +231,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -202,6 +361,42 @@
     <tableColumn id="13" xr3:uid="{BE3B0A33-78E9-44BD-9A7B-54C7A525565B}" name="0">
       <calculatedColumnFormula>Table1[[#This Row],[Points: 0]]/Table1[[#Totals],[Points: 0]]*10*0</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{885EAEC2-D222-4235-A796-2F8B82245935}" name="Table2" displayName="Table2" ref="A1:I14" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{885EAEC2-D222-4235-A796-2F8B82245935}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{476E984D-3029-43B1-A94A-F840A45E05B5}" name="Categories"/>
+    <tableColumn id="8" xr3:uid="{70C4DCE5-CD05-4F49-A262-B2560EB85287}" name="Example5Dice"/>
+    <tableColumn id="9" xr3:uid="{B0636718-55CF-42F2-AF38-DFE62FB93D2A}" name="Example">
+      <calculatedColumnFormula>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{072323CC-08D5-44CE-9139-E3EBF4B09D83}" name="Prop5Dice"/>
+    <tableColumn id="3" xr3:uid="{48E76CB9-2202-4977-BFAD-EA03E3D6CE7B}" name="Prop4Dice"/>
+    <tableColumn id="4" xr3:uid="{23DD030C-8C6E-4322-A932-966D4A9DD3C7}" name="Prop3Dice"/>
+    <tableColumn id="5" xr3:uid="{5E089F67-7849-4F74-AE27-F7C1FBDC9A93}" name="Prop2Dice"/>
+    <tableColumn id="6" xr3:uid="{4064ED51-B48B-419C-A3FB-D578B6339215}" name="Prop1Dice"/>
+    <tableColumn id="7" xr3:uid="{19A14583-AE4F-4A9C-97D8-3B28224ACDE2}" name="Slash"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{375FF3E0-6138-4A41-913C-D1A0C59C7F02}" name="Table24" displayName="Table24" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14" xr:uid="{375FF3E0-6138-4A41-913C-D1A0C59C7F02}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8C07628F-9FCF-4C6F-AA32-90242815860D}" name="Categories"/>
+    <tableColumn id="2" xr3:uid="{90443261-7A9C-4C42-AA37-698D2ED3853A}" name="Prop5Dice"/>
+    <tableColumn id="3" xr3:uid="{87EA7FBA-74AE-4549-9241-CA7D7D16D6B3}" name="Prop4Dice"/>
+    <tableColumn id="4" xr3:uid="{1A8D89C1-214D-4FC5-BEF2-E3545E3BAFBB}" name="Prop3Dice"/>
+    <tableColumn id="5" xr3:uid="{22E5DB89-B43C-4CEC-B7F7-AAF78B3915F4}" name="Prop2Dice"/>
+    <tableColumn id="6" xr3:uid="{5FE46384-9090-43A6-B48B-65DD54A9C637}" name="Prop1Dice"/>
+    <tableColumn id="7" xr3:uid="{281D1893-AD2A-42C8-B980-95441929B742}" name="Slash"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -506,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFD4286-0AF7-410E-9675-FECB4EDF8E8D}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,4 +1403,774 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969BDC67-85F2-46D7-ADEA-2145FB527615}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>2.5758493744782518</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>3.6428011200173973</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>4.4615019892408432</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>5.1516987489565036</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>5.7597743011336817</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>6.3095166217389433</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.23626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>6.3095166217389433</v>
+      </c>
+      <c r="D8">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>6.3095166217389433</v>
+      </c>
+      <c r="D9">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>30.119880477850508</v>
+      </c>
+      <c r="D10">
+        <v>0.36288288000000002</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>42.968906548805734</v>
+      </c>
+      <c r="D11">
+        <v>0.61544231000000005</v>
+      </c>
+      <c r="E11">
+        <v>0.61544231000000005</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>32.316869897934112</v>
+      </c>
+      <c r="D12">
+        <v>0.26109502000000001</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>14.248309373395848</v>
+      </c>
+      <c r="D13">
+        <v>4.0602864000000002E-2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f>SQRT(Table2[[#This Row],[Example5Dice]]*Table2[[#This Row],[Prop5Dice]])*10</f>
+        <v>3.5135452181521725</v>
+      </c>
+      <c r="D14">
+        <v>4.1149999999999997E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.20713E-2</v>
+      </c>
+      <c r="F14">
+        <v>6.1952E-2</v>
+      </c>
+      <c r="G14">
+        <v>6.8269999999999997E-2</v>
+      </c>
+      <c r="H14">
+        <v>1.8600000000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2:H14">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D467981C-C9C5-4BD3-894E-23220382F698}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G4">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G5">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G6">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.34338999999999997</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.23626</v>
+      </c>
+      <c r="G7">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>1.3270000000000001E-2</v>
+      </c>
+      <c r="C9">
+        <v>9.1149999999999995E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.25041999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>0.36288288000000002</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>0.61544231000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.61544231000000005</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0.26109502000000001</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>4.0602864000000002E-2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>4.1149999999999997E-3</v>
+      </c>
+      <c r="C14">
+        <v>1.20713E-2</v>
+      </c>
+      <c r="D14">
+        <v>6.1952E-2</v>
+      </c>
+      <c r="E14">
+        <v>6.8269999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <v>1.8600000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <v>-60</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:F14">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>